<commit_message>
updated login test data file
</commit_message>
<xml_diff>
--- a/testData/Opencart_loginData.xlsx
+++ b/testData/Opencart_loginData.xlsx
@@ -418,7 +418,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,7 +468,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>